<commit_message>
Correcciones + vista link
</commit_message>
<xml_diff>
--- a/back-end/Web Dinamico 2/MRVMinem/Documentos/1.1 Plantilla_Etiquetado_de_eficiencia_ Calentadores_ agua_electrico.xlsx
+++ b/back-end/Web Dinamico 2/MRVMinem/Documentos/1.1 Plantilla_Etiquetado_de_eficiencia_ Calentadores_ agua_electrico.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Dell\Desktop\Nuevas  Plantillas con alfonso\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Dell\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{286EA8FC-AF9D-481D-88A1-05F4F110F989}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{DAC69B16-0844-49A2-81F1-B95B02FE940B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" xr2:uid="{0FF7017A-1C1F-4F31-834A-BE5FD5CEB108}"/>
   </bookViews>
@@ -159,25 +159,25 @@
     <t xml:space="preserve">Capacidad Calentador </t>
   </si>
   <si>
-    <t>Año en que se compró el equipo. Seleccione de la  lista desplegable</t>
-  </si>
-  <si>
     <t>Capacidad (L)</t>
-  </si>
-  <si>
-    <t>Etiqueta del equipo anterior o reemplazado. Seleccione de lista desplegable</t>
-  </si>
-  <si>
-    <t>Etiqueta del equipo nuevo. Seleccione de lista desplegable</t>
   </si>
   <si>
     <t>Número de unidades de este equipo. Inserte su dato.</t>
   </si>
   <si>
-    <t>Mes en que se compro el artefecto. Seleccione el desplegable</t>
+    <t>Año en que se compró el equipo. Seleccione de la  lista desplegable.</t>
   </si>
   <si>
-    <t>Capacidad del calentador de agua eléctrico. Seleccione de la lista desplegable</t>
+    <t>Capacidad del calentador de agua eléctrico. Seleccione de la lista desplegable.</t>
+  </si>
+  <si>
+    <t>Etiqueta del equipo anterior o reemplazado. Seleccione de lista desplegable.</t>
+  </si>
+  <si>
+    <t>Etiqueta del equipo nuevo. Seleccione de lista desplegable.</t>
+  </si>
+  <si>
+    <t>Mes en que se compro el artefecto. Seleccione el desplegable.</t>
   </si>
 </sst>
 </file>
@@ -207,18 +207,19 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <b/>
       <sz val="10"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="9"/>
-      <color indexed="81"/>
-      <name val="Tahoma"/>
-      <charset val="1"/>
     </font>
   </fonts>
   <fills count="6">
@@ -343,9 +344,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyProtection="1">
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
@@ -374,7 +372,10 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -694,7 +695,7 @@
   <dimension ref="A1:J311"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H9" sqref="H9"/>
+      <selection activeCell="J11" sqref="J11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -719,7 +720,7 @@
         <v>1</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D1" s="3" t="s">
         <v>1</v>
@@ -744,88 +745,88 @@
       </c>
     </row>
     <row r="2" spans="1:10" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="11" t="s">
-        <v>30</v>
+      <c r="A2" s="21" t="s">
+        <v>32</v>
       </c>
       <c r="B2" s="1"/>
-      <c r="C2" s="11" t="s">
+      <c r="C2" s="21" t="s">
+        <v>33</v>
+      </c>
+      <c r="D2" s="1"/>
+      <c r="E2" s="21" t="s">
+        <v>34</v>
+      </c>
+      <c r="F2" s="1"/>
+      <c r="G2" s="21" t="s">
+        <v>35</v>
+      </c>
+      <c r="H2" s="22" t="s">
+        <v>31</v>
+      </c>
+      <c r="I2" s="1"/>
+      <c r="J2" s="21" t="s">
         <v>36</v>
       </c>
-      <c r="D2" s="1"/>
-      <c r="E2" s="11" t="s">
-        <v>32</v>
-      </c>
-      <c r="F2" s="1"/>
-      <c r="G2" s="11" t="s">
-        <v>33</v>
-      </c>
-      <c r="H2" s="22" t="s">
-        <v>34</v>
-      </c>
-      <c r="I2" s="1"/>
-      <c r="J2" s="11" t="s">
-        <v>35</v>
-      </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A3" s="18">
+      <c r="A3" s="17">
         <v>2014</v>
       </c>
-      <c r="B3" s="18">
+      <c r="B3" s="17">
         <f t="shared" ref="B3:B66" si="0">VLOOKUP(C3,Tabla_Capacidad,2,)</f>
         <v>2</v>
       </c>
-      <c r="C3" s="18">
+      <c r="C3" s="17">
         <v>50</v>
       </c>
-      <c r="D3" s="18">
+      <c r="D3" s="17">
         <f t="shared" ref="D3:D66" si="1">VLOOKUP(E3,Tabla_BAU,2,)</f>
         <v>5</v>
       </c>
-      <c r="E3" s="18" t="s">
+      <c r="E3" s="17" t="s">
         <v>14</v>
       </c>
-      <c r="F3" s="18">
+      <c r="F3" s="17">
         <f t="shared" ref="F3:F66" si="2">VLOOKUP(G3,Tabla_Iniciativa,2,)</f>
         <v>1</v>
       </c>
-      <c r="G3" s="19" t="s">
+      <c r="G3" s="18" t="s">
         <v>10</v>
       </c>
-      <c r="H3" s="20">
+      <c r="H3" s="19">
         <v>7000</v>
       </c>
-      <c r="I3" s="21">
+      <c r="I3" s="20">
         <f t="shared" ref="I3:I66" si="3">VLOOKUP(J3,Tabla_Mes,2,)</f>
         <v>6</v>
       </c>
-      <c r="J3" s="18" t="s">
+      <c r="J3" s="17" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A4" s="12"/>
-      <c r="B4" s="12" t="e">
+      <c r="A4" s="11"/>
+      <c r="B4" s="11" t="e">
         <f t="shared" si="0"/>
         <v>#N/A</v>
       </c>
-      <c r="C4" s="12"/>
-      <c r="D4" s="12" t="e">
+      <c r="C4" s="11"/>
+      <c r="D4" s="11" t="e">
         <f t="shared" si="1"/>
         <v>#N/A</v>
       </c>
-      <c r="E4" s="12"/>
-      <c r="F4" s="12" t="e">
+      <c r="E4" s="11"/>
+      <c r="F4" s="11" t="e">
         <f t="shared" si="2"/>
         <v>#N/A</v>
       </c>
-      <c r="G4" s="15"/>
-      <c r="H4" s="13"/>
-      <c r="I4" s="16" t="e">
+      <c r="G4" s="14"/>
+      <c r="H4" s="12"/>
+      <c r="I4" s="15" t="e">
         <f t="shared" si="3"/>
         <v>#N/A</v>
       </c>
-      <c r="J4" s="12"/>
+      <c r="J4" s="11"/>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" s="10"/>
@@ -844,7 +845,7 @@
         <v>#N/A</v>
       </c>
       <c r="G5" s="10"/>
-      <c r="H5" s="17"/>
+      <c r="H5" s="16"/>
       <c r="I5" s="10" t="e">
         <f t="shared" si="3"/>
         <v>#N/A</v>
@@ -868,7 +869,7 @@
         <v>#N/A</v>
       </c>
       <c r="G6" s="10"/>
-      <c r="H6" s="17"/>
+      <c r="H6" s="16"/>
       <c r="I6" s="10" t="e">
         <f t="shared" si="3"/>
         <v>#N/A</v>
@@ -892,7 +893,7 @@
         <v>#N/A</v>
       </c>
       <c r="G7" s="10"/>
-      <c r="H7" s="17"/>
+      <c r="H7" s="16"/>
       <c r="I7" s="10" t="e">
         <f t="shared" si="3"/>
         <v>#N/A</v>
@@ -916,7 +917,7 @@
         <v>#N/A</v>
       </c>
       <c r="G8" s="10"/>
-      <c r="H8" s="17"/>
+      <c r="H8" s="16"/>
       <c r="I8" s="10" t="e">
         <f t="shared" si="3"/>
         <v>#N/A</v>
@@ -940,7 +941,7 @@
         <v>#N/A</v>
       </c>
       <c r="G9" s="10"/>
-      <c r="H9" s="17"/>
+      <c r="H9" s="16"/>
       <c r="I9" s="10" t="e">
         <f t="shared" si="3"/>
         <v>#N/A</v>
@@ -964,7 +965,7 @@
         <v>#N/A</v>
       </c>
       <c r="G10" s="10"/>
-      <c r="H10" s="17"/>
+      <c r="H10" s="16"/>
       <c r="I10" s="10" t="e">
         <f t="shared" si="3"/>
         <v>#N/A</v>
@@ -988,7 +989,7 @@
         <v>#N/A</v>
       </c>
       <c r="G11" s="10"/>
-      <c r="H11" s="17"/>
+      <c r="H11" s="16"/>
       <c r="I11" s="10" t="e">
         <f t="shared" si="3"/>
         <v>#N/A</v>
@@ -1012,7 +1013,7 @@
         <v>#N/A</v>
       </c>
       <c r="G12" s="10"/>
-      <c r="H12" s="17"/>
+      <c r="H12" s="16"/>
       <c r="I12" s="10" t="e">
         <f t="shared" si="3"/>
         <v>#N/A</v>
@@ -1036,7 +1037,7 @@
         <v>#N/A</v>
       </c>
       <c r="G13" s="10"/>
-      <c r="H13" s="17"/>
+      <c r="H13" s="16"/>
       <c r="I13" s="10" t="e">
         <f t="shared" si="3"/>
         <v>#N/A</v>
@@ -1060,7 +1061,7 @@
         <v>#N/A</v>
       </c>
       <c r="G14" s="10"/>
-      <c r="H14" s="17"/>
+      <c r="H14" s="16"/>
       <c r="I14" s="10" t="e">
         <f t="shared" si="3"/>
         <v>#N/A</v>
@@ -1084,7 +1085,7 @@
         <v>#N/A</v>
       </c>
       <c r="G15" s="10"/>
-      <c r="H15" s="17"/>
+      <c r="H15" s="16"/>
       <c r="I15" s="10" t="e">
         <f t="shared" si="3"/>
         <v>#N/A</v>
@@ -1108,7 +1109,7 @@
         <v>#N/A</v>
       </c>
       <c r="G16" s="10"/>
-      <c r="H16" s="17"/>
+      <c r="H16" s="16"/>
       <c r="I16" s="10" t="e">
         <f t="shared" si="3"/>
         <v>#N/A</v>
@@ -1132,7 +1133,7 @@
         <v>#N/A</v>
       </c>
       <c r="G17" s="10"/>
-      <c r="H17" s="17"/>
+      <c r="H17" s="16"/>
       <c r="I17" s="10" t="e">
         <f t="shared" si="3"/>
         <v>#N/A</v>
@@ -1156,7 +1157,7 @@
         <v>#N/A</v>
       </c>
       <c r="G18" s="10"/>
-      <c r="H18" s="17"/>
+      <c r="H18" s="16"/>
       <c r="I18" s="10" t="e">
         <f t="shared" si="3"/>
         <v>#N/A</v>
@@ -1180,7 +1181,7 @@
         <v>#N/A</v>
       </c>
       <c r="G19" s="10"/>
-      <c r="H19" s="17"/>
+      <c r="H19" s="16"/>
       <c r="I19" s="10" t="e">
         <f t="shared" si="3"/>
         <v>#N/A</v>
@@ -1204,7 +1205,7 @@
         <v>#N/A</v>
       </c>
       <c r="G20" s="10"/>
-      <c r="H20" s="17"/>
+      <c r="H20" s="16"/>
       <c r="I20" s="10" t="e">
         <f t="shared" si="3"/>
         <v>#N/A</v>
@@ -1228,7 +1229,7 @@
         <v>#N/A</v>
       </c>
       <c r="G21" s="10"/>
-      <c r="H21" s="17"/>
+      <c r="H21" s="16"/>
       <c r="I21" s="10" t="e">
         <f t="shared" si="3"/>
         <v>#N/A</v>
@@ -1252,7 +1253,7 @@
         <v>#N/A</v>
       </c>
       <c r="G22" s="10"/>
-      <c r="H22" s="17"/>
+      <c r="H22" s="16"/>
       <c r="I22" s="10" t="e">
         <f t="shared" si="3"/>
         <v>#N/A</v>
@@ -1276,7 +1277,7 @@
         <v>#N/A</v>
       </c>
       <c r="G23" s="10"/>
-      <c r="H23" s="17"/>
+      <c r="H23" s="16"/>
       <c r="I23" s="10" t="e">
         <f t="shared" si="3"/>
         <v>#N/A</v>
@@ -1300,7 +1301,7 @@
         <v>#N/A</v>
       </c>
       <c r="G24" s="10"/>
-      <c r="H24" s="17"/>
+      <c r="H24" s="16"/>
       <c r="I24" s="10" t="e">
         <f t="shared" si="3"/>
         <v>#N/A</v>
@@ -1324,7 +1325,7 @@
         <v>#N/A</v>
       </c>
       <c r="G25" s="10"/>
-      <c r="H25" s="17"/>
+      <c r="H25" s="16"/>
       <c r="I25" s="10" t="e">
         <f t="shared" si="3"/>
         <v>#N/A</v>
@@ -1348,7 +1349,7 @@
         <v>#N/A</v>
       </c>
       <c r="G26" s="10"/>
-      <c r="H26" s="17"/>
+      <c r="H26" s="16"/>
       <c r="I26" s="10" t="e">
         <f t="shared" si="3"/>
         <v>#N/A</v>
@@ -1372,7 +1373,7 @@
         <v>#N/A</v>
       </c>
       <c r="G27" s="10"/>
-      <c r="H27" s="17"/>
+      <c r="H27" s="16"/>
       <c r="I27" s="10" t="e">
         <f t="shared" si="3"/>
         <v>#N/A</v>
@@ -1396,7 +1397,7 @@
         <v>#N/A</v>
       </c>
       <c r="G28" s="10"/>
-      <c r="H28" s="17"/>
+      <c r="H28" s="16"/>
       <c r="I28" s="10" t="e">
         <f t="shared" si="3"/>
         <v>#N/A</v>
@@ -1420,7 +1421,7 @@
         <v>#N/A</v>
       </c>
       <c r="G29" s="10"/>
-      <c r="H29" s="17"/>
+      <c r="H29" s="16"/>
       <c r="I29" s="10" t="e">
         <f t="shared" si="3"/>
         <v>#N/A</v>
@@ -1444,7 +1445,7 @@
         <v>#N/A</v>
       </c>
       <c r="G30" s="10"/>
-      <c r="H30" s="17"/>
+      <c r="H30" s="16"/>
       <c r="I30" s="10" t="e">
         <f t="shared" si="3"/>
         <v>#N/A</v>
@@ -1468,7 +1469,7 @@
         <v>#N/A</v>
       </c>
       <c r="G31" s="10"/>
-      <c r="H31" s="17"/>
+      <c r="H31" s="16"/>
       <c r="I31" s="10" t="e">
         <f t="shared" si="3"/>
         <v>#N/A</v>
@@ -1492,7 +1493,7 @@
         <v>#N/A</v>
       </c>
       <c r="G32" s="10"/>
-      <c r="H32" s="17"/>
+      <c r="H32" s="16"/>
       <c r="I32" s="10" t="e">
         <f t="shared" si="3"/>
         <v>#N/A</v>
@@ -1516,7 +1517,7 @@
         <v>#N/A</v>
       </c>
       <c r="G33" s="10"/>
-      <c r="H33" s="17"/>
+      <c r="H33" s="16"/>
       <c r="I33" s="10" t="e">
         <f t="shared" si="3"/>
         <v>#N/A</v>
@@ -1540,7 +1541,7 @@
         <v>#N/A</v>
       </c>
       <c r="G34" s="10"/>
-      <c r="H34" s="17"/>
+      <c r="H34" s="16"/>
       <c r="I34" s="10" t="e">
         <f t="shared" si="3"/>
         <v>#N/A</v>
@@ -1564,7 +1565,7 @@
         <v>#N/A</v>
       </c>
       <c r="G35" s="10"/>
-      <c r="H35" s="17"/>
+      <c r="H35" s="16"/>
       <c r="I35" s="10" t="e">
         <f t="shared" si="3"/>
         <v>#N/A</v>
@@ -1588,7 +1589,7 @@
         <v>#N/A</v>
       </c>
       <c r="G36" s="10"/>
-      <c r="H36" s="17"/>
+      <c r="H36" s="16"/>
       <c r="I36" s="10" t="e">
         <f t="shared" si="3"/>
         <v>#N/A</v>
@@ -1612,7 +1613,7 @@
         <v>#N/A</v>
       </c>
       <c r="G37" s="10"/>
-      <c r="H37" s="17"/>
+      <c r="H37" s="16"/>
       <c r="I37" s="10" t="e">
         <f t="shared" si="3"/>
         <v>#N/A</v>
@@ -1636,7 +1637,7 @@
         <v>#N/A</v>
       </c>
       <c r="G38" s="10"/>
-      <c r="H38" s="17"/>
+      <c r="H38" s="16"/>
       <c r="I38" s="10" t="e">
         <f t="shared" si="3"/>
         <v>#N/A</v>
@@ -1660,7 +1661,7 @@
         <v>#N/A</v>
       </c>
       <c r="G39" s="10"/>
-      <c r="H39" s="17"/>
+      <c r="H39" s="16"/>
       <c r="I39" s="10" t="e">
         <f t="shared" si="3"/>
         <v>#N/A</v>
@@ -1684,7 +1685,7 @@
         <v>#N/A</v>
       </c>
       <c r="G40" s="10"/>
-      <c r="H40" s="17"/>
+      <c r="H40" s="16"/>
       <c r="I40" s="10" t="e">
         <f t="shared" si="3"/>
         <v>#N/A</v>
@@ -1708,7 +1709,7 @@
         <v>#N/A</v>
       </c>
       <c r="G41" s="10"/>
-      <c r="H41" s="17"/>
+      <c r="H41" s="16"/>
       <c r="I41" s="10" t="e">
         <f t="shared" si="3"/>
         <v>#N/A</v>
@@ -1732,7 +1733,7 @@
         <v>#N/A</v>
       </c>
       <c r="G42" s="10"/>
-      <c r="H42" s="17"/>
+      <c r="H42" s="16"/>
       <c r="I42" s="10" t="e">
         <f t="shared" si="3"/>
         <v>#N/A</v>
@@ -1756,7 +1757,7 @@
         <v>#N/A</v>
       </c>
       <c r="G43" s="10"/>
-      <c r="H43" s="17"/>
+      <c r="H43" s="16"/>
       <c r="I43" s="10" t="e">
         <f t="shared" si="3"/>
         <v>#N/A</v>
@@ -1780,7 +1781,7 @@
         <v>#N/A</v>
       </c>
       <c r="G44" s="10"/>
-      <c r="H44" s="17"/>
+      <c r="H44" s="16"/>
       <c r="I44" s="10" t="e">
         <f t="shared" si="3"/>
         <v>#N/A</v>
@@ -1804,7 +1805,7 @@
         <v>#N/A</v>
       </c>
       <c r="G45" s="10"/>
-      <c r="H45" s="17"/>
+      <c r="H45" s="16"/>
       <c r="I45" s="10" t="e">
         <f t="shared" si="3"/>
         <v>#N/A</v>
@@ -1828,7 +1829,7 @@
         <v>#N/A</v>
       </c>
       <c r="G46" s="10"/>
-      <c r="H46" s="17"/>
+      <c r="H46" s="16"/>
       <c r="I46" s="10" t="e">
         <f t="shared" si="3"/>
         <v>#N/A</v>
@@ -1852,7 +1853,7 @@
         <v>#N/A</v>
       </c>
       <c r="G47" s="10"/>
-      <c r="H47" s="17"/>
+      <c r="H47" s="16"/>
       <c r="I47" s="10" t="e">
         <f t="shared" si="3"/>
         <v>#N/A</v>
@@ -1876,7 +1877,7 @@
         <v>#N/A</v>
       </c>
       <c r="G48" s="10"/>
-      <c r="H48" s="17"/>
+      <c r="H48" s="16"/>
       <c r="I48" s="10" t="e">
         <f t="shared" si="3"/>
         <v>#N/A</v>
@@ -1900,7 +1901,7 @@
         <v>#N/A</v>
       </c>
       <c r="G49" s="10"/>
-      <c r="H49" s="17"/>
+      <c r="H49" s="16"/>
       <c r="I49" s="10" t="e">
         <f t="shared" si="3"/>
         <v>#N/A</v>
@@ -1924,7 +1925,7 @@
         <v>#N/A</v>
       </c>
       <c r="G50" s="10"/>
-      <c r="H50" s="17"/>
+      <c r="H50" s="16"/>
       <c r="I50" s="10" t="e">
         <f t="shared" si="3"/>
         <v>#N/A</v>
@@ -1948,7 +1949,7 @@
         <v>#N/A</v>
       </c>
       <c r="G51" s="10"/>
-      <c r="H51" s="17"/>
+      <c r="H51" s="16"/>
       <c r="I51" s="10" t="e">
         <f t="shared" si="3"/>
         <v>#N/A</v>
@@ -1972,7 +1973,7 @@
         <v>#N/A</v>
       </c>
       <c r="G52" s="10"/>
-      <c r="H52" s="17"/>
+      <c r="H52" s="16"/>
       <c r="I52" s="10" t="e">
         <f t="shared" si="3"/>
         <v>#N/A</v>
@@ -1996,7 +1997,7 @@
         <v>#N/A</v>
       </c>
       <c r="G53" s="10"/>
-      <c r="H53" s="17"/>
+      <c r="H53" s="16"/>
       <c r="I53" s="10" t="e">
         <f t="shared" si="3"/>
         <v>#N/A</v>
@@ -2020,7 +2021,7 @@
         <v>#N/A</v>
       </c>
       <c r="G54" s="10"/>
-      <c r="H54" s="17"/>
+      <c r="H54" s="16"/>
       <c r="I54" s="10" t="e">
         <f t="shared" si="3"/>
         <v>#N/A</v>
@@ -2044,7 +2045,7 @@
         <v>#N/A</v>
       </c>
       <c r="G55" s="10"/>
-      <c r="H55" s="17"/>
+      <c r="H55" s="16"/>
       <c r="I55" s="10" t="e">
         <f t="shared" si="3"/>
         <v>#N/A</v>
@@ -2068,7 +2069,7 @@
         <v>#N/A</v>
       </c>
       <c r="G56" s="10"/>
-      <c r="H56" s="17"/>
+      <c r="H56" s="16"/>
       <c r="I56" s="10" t="e">
         <f t="shared" si="3"/>
         <v>#N/A</v>
@@ -2092,7 +2093,7 @@
         <v>#N/A</v>
       </c>
       <c r="G57" s="10"/>
-      <c r="H57" s="17"/>
+      <c r="H57" s="16"/>
       <c r="I57" s="10" t="e">
         <f t="shared" si="3"/>
         <v>#N/A</v>
@@ -2116,7 +2117,7 @@
         <v>#N/A</v>
       </c>
       <c r="G58" s="10"/>
-      <c r="H58" s="17"/>
+      <c r="H58" s="16"/>
       <c r="I58" s="10" t="e">
         <f t="shared" si="3"/>
         <v>#N/A</v>
@@ -2140,7 +2141,7 @@
         <v>#N/A</v>
       </c>
       <c r="G59" s="10"/>
-      <c r="H59" s="17"/>
+      <c r="H59" s="16"/>
       <c r="I59" s="10" t="e">
         <f t="shared" si="3"/>
         <v>#N/A</v>
@@ -2164,7 +2165,7 @@
         <v>#N/A</v>
       </c>
       <c r="G60" s="10"/>
-      <c r="H60" s="17"/>
+      <c r="H60" s="16"/>
       <c r="I60" s="10" t="e">
         <f t="shared" si="3"/>
         <v>#N/A</v>
@@ -2188,7 +2189,7 @@
         <v>#N/A</v>
       </c>
       <c r="G61" s="10"/>
-      <c r="H61" s="17"/>
+      <c r="H61" s="16"/>
       <c r="I61" s="10" t="e">
         <f t="shared" si="3"/>
         <v>#N/A</v>
@@ -2212,7 +2213,7 @@
         <v>#N/A</v>
       </c>
       <c r="G62" s="10"/>
-      <c r="H62" s="17"/>
+      <c r="H62" s="16"/>
       <c r="I62" s="10" t="e">
         <f t="shared" si="3"/>
         <v>#N/A</v>
@@ -2236,7 +2237,7 @@
         <v>#N/A</v>
       </c>
       <c r="G63" s="10"/>
-      <c r="H63" s="17"/>
+      <c r="H63" s="16"/>
       <c r="I63" s="10" t="e">
         <f t="shared" si="3"/>
         <v>#N/A</v>
@@ -2260,7 +2261,7 @@
         <v>#N/A</v>
       </c>
       <c r="G64" s="10"/>
-      <c r="H64" s="17"/>
+      <c r="H64" s="16"/>
       <c r="I64" s="10" t="e">
         <f t="shared" si="3"/>
         <v>#N/A</v>
@@ -2284,7 +2285,7 @@
         <v>#N/A</v>
       </c>
       <c r="G65" s="10"/>
-      <c r="H65" s="17"/>
+      <c r="H65" s="16"/>
       <c r="I65" s="10" t="e">
         <f t="shared" si="3"/>
         <v>#N/A</v>
@@ -2308,7 +2309,7 @@
         <v>#N/A</v>
       </c>
       <c r="G66" s="10"/>
-      <c r="H66" s="17"/>
+      <c r="H66" s="16"/>
       <c r="I66" s="10" t="e">
         <f t="shared" si="3"/>
         <v>#N/A</v>
@@ -2332,7 +2333,7 @@
         <v>#N/A</v>
       </c>
       <c r="G67" s="10"/>
-      <c r="H67" s="17"/>
+      <c r="H67" s="16"/>
       <c r="I67" s="10" t="e">
         <f t="shared" ref="I67:I130" si="7">VLOOKUP(J67,Tabla_Mes,2,)</f>
         <v>#N/A</v>
@@ -2356,7 +2357,7 @@
         <v>#N/A</v>
       </c>
       <c r="G68" s="10"/>
-      <c r="H68" s="17"/>
+      <c r="H68" s="16"/>
       <c r="I68" s="10" t="e">
         <f t="shared" si="7"/>
         <v>#N/A</v>
@@ -2380,7 +2381,7 @@
         <v>#N/A</v>
       </c>
       <c r="G69" s="10"/>
-      <c r="H69" s="17"/>
+      <c r="H69" s="16"/>
       <c r="I69" s="10" t="e">
         <f t="shared" si="7"/>
         <v>#N/A</v>
@@ -2404,7 +2405,7 @@
         <v>#N/A</v>
       </c>
       <c r="G70" s="10"/>
-      <c r="H70" s="17"/>
+      <c r="H70" s="16"/>
       <c r="I70" s="10" t="e">
         <f t="shared" si="7"/>
         <v>#N/A</v>
@@ -2428,7 +2429,7 @@
         <v>#N/A</v>
       </c>
       <c r="G71" s="10"/>
-      <c r="H71" s="17"/>
+      <c r="H71" s="16"/>
       <c r="I71" s="10" t="e">
         <f t="shared" si="7"/>
         <v>#N/A</v>
@@ -2452,7 +2453,7 @@
         <v>#N/A</v>
       </c>
       <c r="G72" s="10"/>
-      <c r="H72" s="17"/>
+      <c r="H72" s="16"/>
       <c r="I72" s="10" t="e">
         <f t="shared" si="7"/>
         <v>#N/A</v>
@@ -2476,7 +2477,7 @@
         <v>#N/A</v>
       </c>
       <c r="G73" s="10"/>
-      <c r="H73" s="17"/>
+      <c r="H73" s="16"/>
       <c r="I73" s="10" t="e">
         <f t="shared" si="7"/>
         <v>#N/A</v>
@@ -2500,7 +2501,7 @@
         <v>#N/A</v>
       </c>
       <c r="G74" s="10"/>
-      <c r="H74" s="17"/>
+      <c r="H74" s="16"/>
       <c r="I74" s="10" t="e">
         <f t="shared" si="7"/>
         <v>#N/A</v>
@@ -2524,7 +2525,7 @@
         <v>#N/A</v>
       </c>
       <c r="G75" s="10"/>
-      <c r="H75" s="17"/>
+      <c r="H75" s="16"/>
       <c r="I75" s="10" t="e">
         <f t="shared" si="7"/>
         <v>#N/A</v>
@@ -2548,7 +2549,7 @@
         <v>#N/A</v>
       </c>
       <c r="G76" s="10"/>
-      <c r="H76" s="17"/>
+      <c r="H76" s="16"/>
       <c r="I76" s="10" t="e">
         <f t="shared" si="7"/>
         <v>#N/A</v>
@@ -2572,7 +2573,7 @@
         <v>#N/A</v>
       </c>
       <c r="G77" s="10"/>
-      <c r="H77" s="17"/>
+      <c r="H77" s="16"/>
       <c r="I77" s="10" t="e">
         <f t="shared" si="7"/>
         <v>#N/A</v>
@@ -2596,7 +2597,7 @@
         <v>#N/A</v>
       </c>
       <c r="G78" s="10"/>
-      <c r="H78" s="17"/>
+      <c r="H78" s="16"/>
       <c r="I78" s="10" t="e">
         <f t="shared" si="7"/>
         <v>#N/A</v>
@@ -2620,7 +2621,7 @@
         <v>#N/A</v>
       </c>
       <c r="G79" s="10"/>
-      <c r="H79" s="17"/>
+      <c r="H79" s="16"/>
       <c r="I79" s="10" t="e">
         <f t="shared" si="7"/>
         <v>#N/A</v>
@@ -2644,7 +2645,7 @@
         <v>#N/A</v>
       </c>
       <c r="G80" s="10"/>
-      <c r="H80" s="17"/>
+      <c r="H80" s="16"/>
       <c r="I80" s="10" t="e">
         <f t="shared" si="7"/>
         <v>#N/A</v>
@@ -2668,7 +2669,7 @@
         <v>#N/A</v>
       </c>
       <c r="G81" s="10"/>
-      <c r="H81" s="17"/>
+      <c r="H81" s="16"/>
       <c r="I81" s="10" t="e">
         <f t="shared" si="7"/>
         <v>#N/A</v>
@@ -2692,7 +2693,7 @@
         <v>#N/A</v>
       </c>
       <c r="G82" s="10"/>
-      <c r="H82" s="17"/>
+      <c r="H82" s="16"/>
       <c r="I82" s="10" t="e">
         <f t="shared" si="7"/>
         <v>#N/A</v>
@@ -2716,7 +2717,7 @@
         <v>#N/A</v>
       </c>
       <c r="G83" s="10"/>
-      <c r="H83" s="17"/>
+      <c r="H83" s="16"/>
       <c r="I83" s="10" t="e">
         <f t="shared" si="7"/>
         <v>#N/A</v>
@@ -2740,7 +2741,7 @@
         <v>#N/A</v>
       </c>
       <c r="G84" s="10"/>
-      <c r="H84" s="17"/>
+      <c r="H84" s="16"/>
       <c r="I84" s="10" t="e">
         <f t="shared" si="7"/>
         <v>#N/A</v>
@@ -2764,7 +2765,7 @@
         <v>#N/A</v>
       </c>
       <c r="G85" s="10"/>
-      <c r="H85" s="17"/>
+      <c r="H85" s="16"/>
       <c r="I85" s="10" t="e">
         <f t="shared" si="7"/>
         <v>#N/A</v>
@@ -2788,7 +2789,7 @@
         <v>#N/A</v>
       </c>
       <c r="G86" s="10"/>
-      <c r="H86" s="17"/>
+      <c r="H86" s="16"/>
       <c r="I86" s="10" t="e">
         <f t="shared" si="7"/>
         <v>#N/A</v>
@@ -2812,7 +2813,7 @@
         <v>#N/A</v>
       </c>
       <c r="G87" s="10"/>
-      <c r="H87" s="17"/>
+      <c r="H87" s="16"/>
       <c r="I87" s="10" t="e">
         <f t="shared" si="7"/>
         <v>#N/A</v>
@@ -2836,7 +2837,7 @@
         <v>#N/A</v>
       </c>
       <c r="G88" s="10"/>
-      <c r="H88" s="17"/>
+      <c r="H88" s="16"/>
       <c r="I88" s="10" t="e">
         <f t="shared" si="7"/>
         <v>#N/A</v>
@@ -2860,7 +2861,7 @@
         <v>#N/A</v>
       </c>
       <c r="G89" s="10"/>
-      <c r="H89" s="17"/>
+      <c r="H89" s="16"/>
       <c r="I89" s="10" t="e">
         <f t="shared" si="7"/>
         <v>#N/A</v>
@@ -2884,7 +2885,7 @@
         <v>#N/A</v>
       </c>
       <c r="G90" s="10"/>
-      <c r="H90" s="17"/>
+      <c r="H90" s="16"/>
       <c r="I90" s="10" t="e">
         <f t="shared" si="7"/>
         <v>#N/A</v>
@@ -2908,7 +2909,7 @@
         <v>#N/A</v>
       </c>
       <c r="G91" s="10"/>
-      <c r="H91" s="17"/>
+      <c r="H91" s="16"/>
       <c r="I91" s="10" t="e">
         <f t="shared" si="7"/>
         <v>#N/A</v>
@@ -2932,7 +2933,7 @@
         <v>#N/A</v>
       </c>
       <c r="G92" s="10"/>
-      <c r="H92" s="17"/>
+      <c r="H92" s="16"/>
       <c r="I92" s="10" t="e">
         <f t="shared" si="7"/>
         <v>#N/A</v>
@@ -2956,7 +2957,7 @@
         <v>#N/A</v>
       </c>
       <c r="G93" s="10"/>
-      <c r="H93" s="17"/>
+      <c r="H93" s="16"/>
       <c r="I93" s="10" t="e">
         <f t="shared" si="7"/>
         <v>#N/A</v>
@@ -2980,7 +2981,7 @@
         <v>#N/A</v>
       </c>
       <c r="G94" s="10"/>
-      <c r="H94" s="17"/>
+      <c r="H94" s="16"/>
       <c r="I94" s="10" t="e">
         <f t="shared" si="7"/>
         <v>#N/A</v>
@@ -3004,7 +3005,7 @@
         <v>#N/A</v>
       </c>
       <c r="G95" s="10"/>
-      <c r="H95" s="17"/>
+      <c r="H95" s="16"/>
       <c r="I95" s="10" t="e">
         <f t="shared" si="7"/>
         <v>#N/A</v>
@@ -3028,7 +3029,7 @@
         <v>#N/A</v>
       </c>
       <c r="G96" s="10"/>
-      <c r="H96" s="17"/>
+      <c r="H96" s="16"/>
       <c r="I96" s="10" t="e">
         <f t="shared" si="7"/>
         <v>#N/A</v>
@@ -3052,7 +3053,7 @@
         <v>#N/A</v>
       </c>
       <c r="G97" s="10"/>
-      <c r="H97" s="17"/>
+      <c r="H97" s="16"/>
       <c r="I97" s="10" t="e">
         <f t="shared" si="7"/>
         <v>#N/A</v>
@@ -3076,7 +3077,7 @@
         <v>#N/A</v>
       </c>
       <c r="G98" s="10"/>
-      <c r="H98" s="17"/>
+      <c r="H98" s="16"/>
       <c r="I98" s="10" t="e">
         <f t="shared" si="7"/>
         <v>#N/A</v>
@@ -3100,7 +3101,7 @@
         <v>#N/A</v>
       </c>
       <c r="G99" s="10"/>
-      <c r="H99" s="17"/>
+      <c r="H99" s="16"/>
       <c r="I99" s="10" t="e">
         <f t="shared" si="7"/>
         <v>#N/A</v>
@@ -3124,7 +3125,7 @@
         <v>#N/A</v>
       </c>
       <c r="G100" s="10"/>
-      <c r="H100" s="17"/>
+      <c r="H100" s="16"/>
       <c r="I100" s="10" t="e">
         <f t="shared" si="7"/>
         <v>#N/A</v>
@@ -3148,7 +3149,7 @@
         <v>#N/A</v>
       </c>
       <c r="G101" s="10"/>
-      <c r="H101" s="17"/>
+      <c r="H101" s="16"/>
       <c r="I101" s="10" t="e">
         <f t="shared" si="7"/>
         <v>#N/A</v>
@@ -3172,7 +3173,7 @@
         <v>#N/A</v>
       </c>
       <c r="G102" s="10"/>
-      <c r="H102" s="17"/>
+      <c r="H102" s="16"/>
       <c r="I102" s="10" t="e">
         <f t="shared" si="7"/>
         <v>#N/A</v>
@@ -3196,7 +3197,7 @@
         <v>#N/A</v>
       </c>
       <c r="G103" s="10"/>
-      <c r="H103" s="17"/>
+      <c r="H103" s="16"/>
       <c r="I103" s="10" t="e">
         <f t="shared" si="7"/>
         <v>#N/A</v>
@@ -3220,7 +3221,7 @@
         <v>#N/A</v>
       </c>
       <c r="G104" s="10"/>
-      <c r="H104" s="17"/>
+      <c r="H104" s="16"/>
       <c r="I104" s="10" t="e">
         <f t="shared" si="7"/>
         <v>#N/A</v>
@@ -3244,7 +3245,7 @@
         <v>#N/A</v>
       </c>
       <c r="G105" s="10"/>
-      <c r="H105" s="17"/>
+      <c r="H105" s="16"/>
       <c r="I105" s="10" t="e">
         <f t="shared" si="7"/>
         <v>#N/A</v>
@@ -3268,7 +3269,7 @@
         <v>#N/A</v>
       </c>
       <c r="G106" s="10"/>
-      <c r="H106" s="17"/>
+      <c r="H106" s="16"/>
       <c r="I106" s="10" t="e">
         <f t="shared" si="7"/>
         <v>#N/A</v>
@@ -3292,7 +3293,7 @@
         <v>#N/A</v>
       </c>
       <c r="G107" s="10"/>
-      <c r="H107" s="17"/>
+      <c r="H107" s="16"/>
       <c r="I107" s="10" t="e">
         <f t="shared" si="7"/>
         <v>#N/A</v>
@@ -3316,7 +3317,7 @@
         <v>#N/A</v>
       </c>
       <c r="G108" s="10"/>
-      <c r="H108" s="17"/>
+      <c r="H108" s="16"/>
       <c r="I108" s="10" t="e">
         <f t="shared" si="7"/>
         <v>#N/A</v>
@@ -3340,7 +3341,7 @@
         <v>#N/A</v>
       </c>
       <c r="G109" s="10"/>
-      <c r="H109" s="17"/>
+      <c r="H109" s="16"/>
       <c r="I109" s="10" t="e">
         <f t="shared" si="7"/>
         <v>#N/A</v>
@@ -3364,7 +3365,7 @@
         <v>#N/A</v>
       </c>
       <c r="G110" s="10"/>
-      <c r="H110" s="17"/>
+      <c r="H110" s="16"/>
       <c r="I110" s="10" t="e">
         <f t="shared" si="7"/>
         <v>#N/A</v>
@@ -3388,7 +3389,7 @@
         <v>#N/A</v>
       </c>
       <c r="G111" s="10"/>
-      <c r="H111" s="17"/>
+      <c r="H111" s="16"/>
       <c r="I111" s="10" t="e">
         <f t="shared" si="7"/>
         <v>#N/A</v>
@@ -3412,7 +3413,7 @@
         <v>#N/A</v>
       </c>
       <c r="G112" s="10"/>
-      <c r="H112" s="17"/>
+      <c r="H112" s="16"/>
       <c r="I112" s="10" t="e">
         <f t="shared" si="7"/>
         <v>#N/A</v>
@@ -3436,7 +3437,7 @@
         <v>#N/A</v>
       </c>
       <c r="G113" s="10"/>
-      <c r="H113" s="17"/>
+      <c r="H113" s="16"/>
       <c r="I113" s="10" t="e">
         <f t="shared" si="7"/>
         <v>#N/A</v>
@@ -3460,7 +3461,7 @@
         <v>#N/A</v>
       </c>
       <c r="G114" s="10"/>
-      <c r="H114" s="17"/>
+      <c r="H114" s="16"/>
       <c r="I114" s="10" t="e">
         <f t="shared" si="7"/>
         <v>#N/A</v>
@@ -3484,7 +3485,7 @@
         <v>#N/A</v>
       </c>
       <c r="G115" s="10"/>
-      <c r="H115" s="17"/>
+      <c r="H115" s="16"/>
       <c r="I115" s="10" t="e">
         <f t="shared" si="7"/>
         <v>#N/A</v>
@@ -3508,7 +3509,7 @@
         <v>#N/A</v>
       </c>
       <c r="G116" s="10"/>
-      <c r="H116" s="17"/>
+      <c r="H116" s="16"/>
       <c r="I116" s="10" t="e">
         <f t="shared" si="7"/>
         <v>#N/A</v>
@@ -3532,7 +3533,7 @@
         <v>#N/A</v>
       </c>
       <c r="G117" s="10"/>
-      <c r="H117" s="17"/>
+      <c r="H117" s="16"/>
       <c r="I117" s="10" t="e">
         <f t="shared" si="7"/>
         <v>#N/A</v>
@@ -3556,7 +3557,7 @@
         <v>#N/A</v>
       </c>
       <c r="G118" s="10"/>
-      <c r="H118" s="17"/>
+      <c r="H118" s="16"/>
       <c r="I118" s="10" t="e">
         <f t="shared" si="7"/>
         <v>#N/A</v>
@@ -3580,7 +3581,7 @@
         <v>#N/A</v>
       </c>
       <c r="G119" s="10"/>
-      <c r="H119" s="17"/>
+      <c r="H119" s="16"/>
       <c r="I119" s="10" t="e">
         <f t="shared" si="7"/>
         <v>#N/A</v>
@@ -3604,7 +3605,7 @@
         <v>#N/A</v>
       </c>
       <c r="G120" s="10"/>
-      <c r="H120" s="17"/>
+      <c r="H120" s="16"/>
       <c r="I120" s="10" t="e">
         <f t="shared" si="7"/>
         <v>#N/A</v>
@@ -3628,7 +3629,7 @@
         <v>#N/A</v>
       </c>
       <c r="G121" s="10"/>
-      <c r="H121" s="17"/>
+      <c r="H121" s="16"/>
       <c r="I121" s="10" t="e">
         <f t="shared" si="7"/>
         <v>#N/A</v>
@@ -3652,7 +3653,7 @@
         <v>#N/A</v>
       </c>
       <c r="G122" s="10"/>
-      <c r="H122" s="17"/>
+      <c r="H122" s="16"/>
       <c r="I122" s="10" t="e">
         <f t="shared" si="7"/>
         <v>#N/A</v>
@@ -3676,7 +3677,7 @@
         <v>#N/A</v>
       </c>
       <c r="G123" s="10"/>
-      <c r="H123" s="17"/>
+      <c r="H123" s="16"/>
       <c r="I123" s="10" t="e">
         <f t="shared" si="7"/>
         <v>#N/A</v>
@@ -3700,7 +3701,7 @@
         <v>#N/A</v>
       </c>
       <c r="G124" s="10"/>
-      <c r="H124" s="17"/>
+      <c r="H124" s="16"/>
       <c r="I124" s="10" t="e">
         <f t="shared" si="7"/>
         <v>#N/A</v>
@@ -3724,7 +3725,7 @@
         <v>#N/A</v>
       </c>
       <c r="G125" s="10"/>
-      <c r="H125" s="17"/>
+      <c r="H125" s="16"/>
       <c r="I125" s="10" t="e">
         <f t="shared" si="7"/>
         <v>#N/A</v>
@@ -3748,7 +3749,7 @@
         <v>#N/A</v>
       </c>
       <c r="G126" s="10"/>
-      <c r="H126" s="17"/>
+      <c r="H126" s="16"/>
       <c r="I126" s="10" t="e">
         <f t="shared" si="7"/>
         <v>#N/A</v>
@@ -3772,7 +3773,7 @@
         <v>#N/A</v>
       </c>
       <c r="G127" s="10"/>
-      <c r="H127" s="17"/>
+      <c r="H127" s="16"/>
       <c r="I127" s="10" t="e">
         <f t="shared" si="7"/>
         <v>#N/A</v>
@@ -3796,7 +3797,7 @@
         <v>#N/A</v>
       </c>
       <c r="G128" s="10"/>
-      <c r="H128" s="17"/>
+      <c r="H128" s="16"/>
       <c r="I128" s="10" t="e">
         <f t="shared" si="7"/>
         <v>#N/A</v>
@@ -3820,7 +3821,7 @@
         <v>#N/A</v>
       </c>
       <c r="G129" s="10"/>
-      <c r="H129" s="17"/>
+      <c r="H129" s="16"/>
       <c r="I129" s="10" t="e">
         <f t="shared" si="7"/>
         <v>#N/A</v>
@@ -3844,7 +3845,7 @@
         <v>#N/A</v>
       </c>
       <c r="G130" s="10"/>
-      <c r="H130" s="17"/>
+      <c r="H130" s="16"/>
       <c r="I130" s="10" t="e">
         <f t="shared" si="7"/>
         <v>#N/A</v>
@@ -3868,7 +3869,7 @@
         <v>#N/A</v>
       </c>
       <c r="G131" s="10"/>
-      <c r="H131" s="17"/>
+      <c r="H131" s="16"/>
       <c r="I131" s="10" t="e">
         <f t="shared" ref="I131:I194" si="11">VLOOKUP(J131,Tabla_Mes,2,)</f>
         <v>#N/A</v>
@@ -3892,7 +3893,7 @@
         <v>#N/A</v>
       </c>
       <c r="G132" s="10"/>
-      <c r="H132" s="17"/>
+      <c r="H132" s="16"/>
       <c r="I132" s="10" t="e">
         <f t="shared" si="11"/>
         <v>#N/A</v>
@@ -3916,7 +3917,7 @@
         <v>#N/A</v>
       </c>
       <c r="G133" s="10"/>
-      <c r="H133" s="17"/>
+      <c r="H133" s="16"/>
       <c r="I133" s="10" t="e">
         <f t="shared" si="11"/>
         <v>#N/A</v>
@@ -3940,7 +3941,7 @@
         <v>#N/A</v>
       </c>
       <c r="G134" s="10"/>
-      <c r="H134" s="17"/>
+      <c r="H134" s="16"/>
       <c r="I134" s="10" t="e">
         <f t="shared" si="11"/>
         <v>#N/A</v>
@@ -3964,7 +3965,7 @@
         <v>#N/A</v>
       </c>
       <c r="G135" s="10"/>
-      <c r="H135" s="17"/>
+      <c r="H135" s="16"/>
       <c r="I135" s="10" t="e">
         <f t="shared" si="11"/>
         <v>#N/A</v>
@@ -3988,7 +3989,7 @@
         <v>#N/A</v>
       </c>
       <c r="G136" s="10"/>
-      <c r="H136" s="17"/>
+      <c r="H136" s="16"/>
       <c r="I136" s="10" t="e">
         <f t="shared" si="11"/>
         <v>#N/A</v>
@@ -4012,7 +4013,7 @@
         <v>#N/A</v>
       </c>
       <c r="G137" s="10"/>
-      <c r="H137" s="17"/>
+      <c r="H137" s="16"/>
       <c r="I137" s="10" t="e">
         <f t="shared" si="11"/>
         <v>#N/A</v>
@@ -4036,7 +4037,7 @@
         <v>#N/A</v>
       </c>
       <c r="G138" s="10"/>
-      <c r="H138" s="17"/>
+      <c r="H138" s="16"/>
       <c r="I138" s="10" t="e">
         <f t="shared" si="11"/>
         <v>#N/A</v>
@@ -4060,7 +4061,7 @@
         <v>#N/A</v>
       </c>
       <c r="G139" s="10"/>
-      <c r="H139" s="17"/>
+      <c r="H139" s="16"/>
       <c r="I139" s="10" t="e">
         <f t="shared" si="11"/>
         <v>#N/A</v>
@@ -4084,7 +4085,7 @@
         <v>#N/A</v>
       </c>
       <c r="G140" s="10"/>
-      <c r="H140" s="17"/>
+      <c r="H140" s="16"/>
       <c r="I140" s="10" t="e">
         <f t="shared" si="11"/>
         <v>#N/A</v>
@@ -4108,7 +4109,7 @@
         <v>#N/A</v>
       </c>
       <c r="G141" s="10"/>
-      <c r="H141" s="17"/>
+      <c r="H141" s="16"/>
       <c r="I141" s="10" t="e">
         <f t="shared" si="11"/>
         <v>#N/A</v>
@@ -4132,7 +4133,7 @@
         <v>#N/A</v>
       </c>
       <c r="G142" s="10"/>
-      <c r="H142" s="17"/>
+      <c r="H142" s="16"/>
       <c r="I142" s="10" t="e">
         <f t="shared" si="11"/>
         <v>#N/A</v>
@@ -4156,7 +4157,7 @@
         <v>#N/A</v>
       </c>
       <c r="G143" s="10"/>
-      <c r="H143" s="17"/>
+      <c r="H143" s="16"/>
       <c r="I143" s="10" t="e">
         <f t="shared" si="11"/>
         <v>#N/A</v>
@@ -4180,7 +4181,7 @@
         <v>#N/A</v>
       </c>
       <c r="G144" s="10"/>
-      <c r="H144" s="17"/>
+      <c r="H144" s="16"/>
       <c r="I144" s="10" t="e">
         <f t="shared" si="11"/>
         <v>#N/A</v>
@@ -4204,7 +4205,7 @@
         <v>#N/A</v>
       </c>
       <c r="G145" s="10"/>
-      <c r="H145" s="17"/>
+      <c r="H145" s="16"/>
       <c r="I145" s="10" t="e">
         <f t="shared" si="11"/>
         <v>#N/A</v>
@@ -4228,7 +4229,7 @@
         <v>#N/A</v>
       </c>
       <c r="G146" s="10"/>
-      <c r="H146" s="17"/>
+      <c r="H146" s="16"/>
       <c r="I146" s="10" t="e">
         <f t="shared" si="11"/>
         <v>#N/A</v>
@@ -4252,7 +4253,7 @@
         <v>#N/A</v>
       </c>
       <c r="G147" s="10"/>
-      <c r="H147" s="17"/>
+      <c r="H147" s="16"/>
       <c r="I147" s="10" t="e">
         <f t="shared" si="11"/>
         <v>#N/A</v>
@@ -4276,7 +4277,7 @@
         <v>#N/A</v>
       </c>
       <c r="G148" s="10"/>
-      <c r="H148" s="17"/>
+      <c r="H148" s="16"/>
       <c r="I148" s="10" t="e">
         <f t="shared" si="11"/>
         <v>#N/A</v>
@@ -4300,7 +4301,7 @@
         <v>#N/A</v>
       </c>
       <c r="G149" s="10"/>
-      <c r="H149" s="17"/>
+      <c r="H149" s="16"/>
       <c r="I149" s="10" t="e">
         <f t="shared" si="11"/>
         <v>#N/A</v>
@@ -4324,7 +4325,7 @@
         <v>#N/A</v>
       </c>
       <c r="G150" s="10"/>
-      <c r="H150" s="17"/>
+      <c r="H150" s="16"/>
       <c r="I150" s="10" t="e">
         <f t="shared" si="11"/>
         <v>#N/A</v>
@@ -4348,7 +4349,7 @@
         <v>#N/A</v>
       </c>
       <c r="G151" s="10"/>
-      <c r="H151" s="17"/>
+      <c r="H151" s="16"/>
       <c r="I151" s="10" t="e">
         <f t="shared" si="11"/>
         <v>#N/A</v>
@@ -4372,7 +4373,7 @@
         <v>#N/A</v>
       </c>
       <c r="G152" s="10"/>
-      <c r="H152" s="17"/>
+      <c r="H152" s="16"/>
       <c r="I152" s="10" t="e">
         <f t="shared" si="11"/>
         <v>#N/A</v>
@@ -4396,7 +4397,7 @@
         <v>#N/A</v>
       </c>
       <c r="G153" s="10"/>
-      <c r="H153" s="17"/>
+      <c r="H153" s="16"/>
       <c r="I153" s="10" t="e">
         <f t="shared" si="11"/>
         <v>#N/A</v>
@@ -4420,7 +4421,7 @@
         <v>#N/A</v>
       </c>
       <c r="G154" s="10"/>
-      <c r="H154" s="17"/>
+      <c r="H154" s="16"/>
       <c r="I154" s="10" t="e">
         <f t="shared" si="11"/>
         <v>#N/A</v>
@@ -4444,7 +4445,7 @@
         <v>#N/A</v>
       </c>
       <c r="G155" s="10"/>
-      <c r="H155" s="17"/>
+      <c r="H155" s="16"/>
       <c r="I155" s="10" t="e">
         <f t="shared" si="11"/>
         <v>#N/A</v>
@@ -4468,7 +4469,7 @@
         <v>#N/A</v>
       </c>
       <c r="G156" s="10"/>
-      <c r="H156" s="17"/>
+      <c r="H156" s="16"/>
       <c r="I156" s="10" t="e">
         <f t="shared" si="11"/>
         <v>#N/A</v>
@@ -4492,7 +4493,7 @@
         <v>#N/A</v>
       </c>
       <c r="G157" s="10"/>
-      <c r="H157" s="17"/>
+      <c r="H157" s="16"/>
       <c r="I157" s="10" t="e">
         <f t="shared" si="11"/>
         <v>#N/A</v>
@@ -4516,7 +4517,7 @@
         <v>#N/A</v>
       </c>
       <c r="G158" s="10"/>
-      <c r="H158" s="17"/>
+      <c r="H158" s="16"/>
       <c r="I158" s="10" t="e">
         <f t="shared" si="11"/>
         <v>#N/A</v>
@@ -4540,7 +4541,7 @@
         <v>#N/A</v>
       </c>
       <c r="G159" s="10"/>
-      <c r="H159" s="17"/>
+      <c r="H159" s="16"/>
       <c r="I159" s="10" t="e">
         <f t="shared" si="11"/>
         <v>#N/A</v>
@@ -4564,7 +4565,7 @@
         <v>#N/A</v>
       </c>
       <c r="G160" s="10"/>
-      <c r="H160" s="17"/>
+      <c r="H160" s="16"/>
       <c r="I160" s="10" t="e">
         <f t="shared" si="11"/>
         <v>#N/A</v>
@@ -4588,7 +4589,7 @@
         <v>#N/A</v>
       </c>
       <c r="G161" s="10"/>
-      <c r="H161" s="17"/>
+      <c r="H161" s="16"/>
       <c r="I161" s="10" t="e">
         <f t="shared" si="11"/>
         <v>#N/A</v>
@@ -4612,7 +4613,7 @@
         <v>#N/A</v>
       </c>
       <c r="G162" s="10"/>
-      <c r="H162" s="17"/>
+      <c r="H162" s="16"/>
       <c r="I162" s="10" t="e">
         <f t="shared" si="11"/>
         <v>#N/A</v>
@@ -4636,7 +4637,7 @@
         <v>#N/A</v>
       </c>
       <c r="G163" s="10"/>
-      <c r="H163" s="17"/>
+      <c r="H163" s="16"/>
       <c r="I163" s="10" t="e">
         <f t="shared" si="11"/>
         <v>#N/A</v>
@@ -4660,7 +4661,7 @@
         <v>#N/A</v>
       </c>
       <c r="G164" s="10"/>
-      <c r="H164" s="17"/>
+      <c r="H164" s="16"/>
       <c r="I164" s="10" t="e">
         <f t="shared" si="11"/>
         <v>#N/A</v>
@@ -4684,7 +4685,7 @@
         <v>#N/A</v>
       </c>
       <c r="G165" s="10"/>
-      <c r="H165" s="17"/>
+      <c r="H165" s="16"/>
       <c r="I165" s="10" t="e">
         <f t="shared" si="11"/>
         <v>#N/A</v>
@@ -4708,7 +4709,7 @@
         <v>#N/A</v>
       </c>
       <c r="G166" s="10"/>
-      <c r="H166" s="17"/>
+      <c r="H166" s="16"/>
       <c r="I166" s="10" t="e">
         <f t="shared" si="11"/>
         <v>#N/A</v>
@@ -4732,7 +4733,7 @@
         <v>#N/A</v>
       </c>
       <c r="G167" s="10"/>
-      <c r="H167" s="17"/>
+      <c r="H167" s="16"/>
       <c r="I167" s="10" t="e">
         <f t="shared" si="11"/>
         <v>#N/A</v>
@@ -4756,7 +4757,7 @@
         <v>#N/A</v>
       </c>
       <c r="G168" s="10"/>
-      <c r="H168" s="17"/>
+      <c r="H168" s="16"/>
       <c r="I168" s="10" t="e">
         <f t="shared" si="11"/>
         <v>#N/A</v>
@@ -4780,7 +4781,7 @@
         <v>#N/A</v>
       </c>
       <c r="G169" s="10"/>
-      <c r="H169" s="17"/>
+      <c r="H169" s="16"/>
       <c r="I169" s="10" t="e">
         <f t="shared" si="11"/>
         <v>#N/A</v>
@@ -4804,7 +4805,7 @@
         <v>#N/A</v>
       </c>
       <c r="G170" s="10"/>
-      <c r="H170" s="17"/>
+      <c r="H170" s="16"/>
       <c r="I170" s="10" t="e">
         <f t="shared" si="11"/>
         <v>#N/A</v>
@@ -4828,7 +4829,7 @@
         <v>#N/A</v>
       </c>
       <c r="G171" s="10"/>
-      <c r="H171" s="17"/>
+      <c r="H171" s="16"/>
       <c r="I171" s="10" t="e">
         <f t="shared" si="11"/>
         <v>#N/A</v>
@@ -4852,7 +4853,7 @@
         <v>#N/A</v>
       </c>
       <c r="G172" s="10"/>
-      <c r="H172" s="17"/>
+      <c r="H172" s="16"/>
       <c r="I172" s="10" t="e">
         <f t="shared" si="11"/>
         <v>#N/A</v>
@@ -4876,7 +4877,7 @@
         <v>#N/A</v>
       </c>
       <c r="G173" s="10"/>
-      <c r="H173" s="17"/>
+      <c r="H173" s="16"/>
       <c r="I173" s="10" t="e">
         <f t="shared" si="11"/>
         <v>#N/A</v>
@@ -4900,7 +4901,7 @@
         <v>#N/A</v>
       </c>
       <c r="G174" s="10"/>
-      <c r="H174" s="17"/>
+      <c r="H174" s="16"/>
       <c r="I174" s="10" t="e">
         <f t="shared" si="11"/>
         <v>#N/A</v>
@@ -4924,7 +4925,7 @@
         <v>#N/A</v>
       </c>
       <c r="G175" s="10"/>
-      <c r="H175" s="17"/>
+      <c r="H175" s="16"/>
       <c r="I175" s="10" t="e">
         <f t="shared" si="11"/>
         <v>#N/A</v>
@@ -4948,7 +4949,7 @@
         <v>#N/A</v>
       </c>
       <c r="G176" s="10"/>
-      <c r="H176" s="17"/>
+      <c r="H176" s="16"/>
       <c r="I176" s="10" t="e">
         <f t="shared" si="11"/>
         <v>#N/A</v>
@@ -4972,7 +4973,7 @@
         <v>#N/A</v>
       </c>
       <c r="G177" s="10"/>
-      <c r="H177" s="17"/>
+      <c r="H177" s="16"/>
       <c r="I177" s="10" t="e">
         <f t="shared" si="11"/>
         <v>#N/A</v>
@@ -4996,7 +4997,7 @@
         <v>#N/A</v>
       </c>
       <c r="G178" s="10"/>
-      <c r="H178" s="17"/>
+      <c r="H178" s="16"/>
       <c r="I178" s="10" t="e">
         <f t="shared" si="11"/>
         <v>#N/A</v>
@@ -5020,7 +5021,7 @@
         <v>#N/A</v>
       </c>
       <c r="G179" s="10"/>
-      <c r="H179" s="17"/>
+      <c r="H179" s="16"/>
       <c r="I179" s="10" t="e">
         <f t="shared" si="11"/>
         <v>#N/A</v>
@@ -5044,7 +5045,7 @@
         <v>#N/A</v>
       </c>
       <c r="G180" s="10"/>
-      <c r="H180" s="17"/>
+      <c r="H180" s="16"/>
       <c r="I180" s="10" t="e">
         <f t="shared" si="11"/>
         <v>#N/A</v>
@@ -5068,7 +5069,7 @@
         <v>#N/A</v>
       </c>
       <c r="G181" s="10"/>
-      <c r="H181" s="17"/>
+      <c r="H181" s="16"/>
       <c r="I181" s="10" t="e">
         <f t="shared" si="11"/>
         <v>#N/A</v>
@@ -5092,7 +5093,7 @@
         <v>#N/A</v>
       </c>
       <c r="G182" s="10"/>
-      <c r="H182" s="17"/>
+      <c r="H182" s="16"/>
       <c r="I182" s="10" t="e">
         <f t="shared" si="11"/>
         <v>#N/A</v>
@@ -5116,7 +5117,7 @@
         <v>#N/A</v>
       </c>
       <c r="G183" s="10"/>
-      <c r="H183" s="17"/>
+      <c r="H183" s="16"/>
       <c r="I183" s="10" t="e">
         <f t="shared" si="11"/>
         <v>#N/A</v>
@@ -5140,7 +5141,7 @@
         <v>#N/A</v>
       </c>
       <c r="G184" s="10"/>
-      <c r="H184" s="17"/>
+      <c r="H184" s="16"/>
       <c r="I184" s="10" t="e">
         <f t="shared" si="11"/>
         <v>#N/A</v>
@@ -5164,7 +5165,7 @@
         <v>#N/A</v>
       </c>
       <c r="G185" s="10"/>
-      <c r="H185" s="17"/>
+      <c r="H185" s="16"/>
       <c r="I185" s="10" t="e">
         <f t="shared" si="11"/>
         <v>#N/A</v>
@@ -5188,7 +5189,7 @@
         <v>#N/A</v>
       </c>
       <c r="G186" s="10"/>
-      <c r="H186" s="17"/>
+      <c r="H186" s="16"/>
       <c r="I186" s="10" t="e">
         <f t="shared" si="11"/>
         <v>#N/A</v>
@@ -5212,7 +5213,7 @@
         <v>#N/A</v>
       </c>
       <c r="G187" s="10"/>
-      <c r="H187" s="17"/>
+      <c r="H187" s="16"/>
       <c r="I187" s="10" t="e">
         <f t="shared" si="11"/>
         <v>#N/A</v>
@@ -5236,7 +5237,7 @@
         <v>#N/A</v>
       </c>
       <c r="G188" s="10"/>
-      <c r="H188" s="17"/>
+      <c r="H188" s="16"/>
       <c r="I188" s="10" t="e">
         <f t="shared" si="11"/>
         <v>#N/A</v>
@@ -5260,7 +5261,7 @@
         <v>#N/A</v>
       </c>
       <c r="G189" s="10"/>
-      <c r="H189" s="17"/>
+      <c r="H189" s="16"/>
       <c r="I189" s="10" t="e">
         <f t="shared" si="11"/>
         <v>#N/A</v>
@@ -5284,7 +5285,7 @@
         <v>#N/A</v>
       </c>
       <c r="G190" s="10"/>
-      <c r="H190" s="17"/>
+      <c r="H190" s="16"/>
       <c r="I190" s="10" t="e">
         <f t="shared" si="11"/>
         <v>#N/A</v>
@@ -5308,7 +5309,7 @@
         <v>#N/A</v>
       </c>
       <c r="G191" s="10"/>
-      <c r="H191" s="17"/>
+      <c r="H191" s="16"/>
       <c r="I191" s="10" t="e">
         <f t="shared" si="11"/>
         <v>#N/A</v>
@@ -5332,7 +5333,7 @@
         <v>#N/A</v>
       </c>
       <c r="G192" s="10"/>
-      <c r="H192" s="17"/>
+      <c r="H192" s="16"/>
       <c r="I192" s="10" t="e">
         <f t="shared" si="11"/>
         <v>#N/A</v>
@@ -5356,7 +5357,7 @@
         <v>#N/A</v>
       </c>
       <c r="G193" s="10"/>
-      <c r="H193" s="17"/>
+      <c r="H193" s="16"/>
       <c r="I193" s="10" t="e">
         <f t="shared" si="11"/>
         <v>#N/A</v>
@@ -5380,7 +5381,7 @@
         <v>#N/A</v>
       </c>
       <c r="G194" s="10"/>
-      <c r="H194" s="17"/>
+      <c r="H194" s="16"/>
       <c r="I194" s="10" t="e">
         <f t="shared" si="11"/>
         <v>#N/A</v>
@@ -5404,7 +5405,7 @@
         <v>#N/A</v>
       </c>
       <c r="G195" s="10"/>
-      <c r="H195" s="17"/>
+      <c r="H195" s="16"/>
       <c r="I195" s="10" t="e">
         <f t="shared" ref="I195:I258" si="15">VLOOKUP(J195,Tabla_Mes,2,)</f>
         <v>#N/A</v>
@@ -5428,7 +5429,7 @@
         <v>#N/A</v>
       </c>
       <c r="G196" s="10"/>
-      <c r="H196" s="17"/>
+      <c r="H196" s="16"/>
       <c r="I196" s="10" t="e">
         <f t="shared" si="15"/>
         <v>#N/A</v>
@@ -5452,7 +5453,7 @@
         <v>#N/A</v>
       </c>
       <c r="G197" s="10"/>
-      <c r="H197" s="17"/>
+      <c r="H197" s="16"/>
       <c r="I197" s="10" t="e">
         <f t="shared" si="15"/>
         <v>#N/A</v>
@@ -5476,7 +5477,7 @@
         <v>#N/A</v>
       </c>
       <c r="G198" s="10"/>
-      <c r="H198" s="17"/>
+      <c r="H198" s="16"/>
       <c r="I198" s="10" t="e">
         <f t="shared" si="15"/>
         <v>#N/A</v>
@@ -5500,7 +5501,7 @@
         <v>#N/A</v>
       </c>
       <c r="G199" s="10"/>
-      <c r="H199" s="17"/>
+      <c r="H199" s="16"/>
       <c r="I199" s="10" t="e">
         <f t="shared" si="15"/>
         <v>#N/A</v>
@@ -5524,7 +5525,7 @@
         <v>#N/A</v>
       </c>
       <c r="G200" s="10"/>
-      <c r="H200" s="17"/>
+      <c r="H200" s="16"/>
       <c r="I200" s="10" t="e">
         <f t="shared" si="15"/>
         <v>#N/A</v>
@@ -5548,7 +5549,7 @@
         <v>#N/A</v>
       </c>
       <c r="G201" s="10"/>
-      <c r="H201" s="17"/>
+      <c r="H201" s="16"/>
       <c r="I201" s="10" t="e">
         <f t="shared" si="15"/>
         <v>#N/A</v>
@@ -5572,7 +5573,7 @@
         <v>#N/A</v>
       </c>
       <c r="G202" s="10"/>
-      <c r="H202" s="17"/>
+      <c r="H202" s="16"/>
       <c r="I202" s="10" t="e">
         <f t="shared" si="15"/>
         <v>#N/A</v>
@@ -5596,7 +5597,7 @@
         <v>#N/A</v>
       </c>
       <c r="G203" s="10"/>
-      <c r="H203" s="17"/>
+      <c r="H203" s="16"/>
       <c r="I203" s="10" t="e">
         <f t="shared" si="15"/>
         <v>#N/A</v>
@@ -5620,7 +5621,7 @@
         <v>#N/A</v>
       </c>
       <c r="G204" s="10"/>
-      <c r="H204" s="17"/>
+      <c r="H204" s="16"/>
       <c r="I204" s="10" t="e">
         <f t="shared" si="15"/>
         <v>#N/A</v>
@@ -5644,7 +5645,7 @@
         <v>#N/A</v>
       </c>
       <c r="G205" s="10"/>
-      <c r="H205" s="17"/>
+      <c r="H205" s="16"/>
       <c r="I205" s="10" t="e">
         <f t="shared" si="15"/>
         <v>#N/A</v>
@@ -5668,7 +5669,7 @@
         <v>#N/A</v>
       </c>
       <c r="G206" s="10"/>
-      <c r="H206" s="17"/>
+      <c r="H206" s="16"/>
       <c r="I206" s="10" t="e">
         <f t="shared" si="15"/>
         <v>#N/A</v>
@@ -5692,7 +5693,7 @@
         <v>#N/A</v>
       </c>
       <c r="G207" s="10"/>
-      <c r="H207" s="17"/>
+      <c r="H207" s="16"/>
       <c r="I207" s="10" t="e">
         <f t="shared" si="15"/>
         <v>#N/A</v>
@@ -5716,7 +5717,7 @@
         <v>#N/A</v>
       </c>
       <c r="G208" s="10"/>
-      <c r="H208" s="17"/>
+      <c r="H208" s="16"/>
       <c r="I208" s="10" t="e">
         <f t="shared" si="15"/>
         <v>#N/A</v>
@@ -5740,7 +5741,7 @@
         <v>#N/A</v>
       </c>
       <c r="G209" s="10"/>
-      <c r="H209" s="17"/>
+      <c r="H209" s="16"/>
       <c r="I209" s="10" t="e">
         <f t="shared" si="15"/>
         <v>#N/A</v>
@@ -5764,7 +5765,7 @@
         <v>#N/A</v>
       </c>
       <c r="G210" s="10"/>
-      <c r="H210" s="17"/>
+      <c r="H210" s="16"/>
       <c r="I210" s="10" t="e">
         <f t="shared" si="15"/>
         <v>#N/A</v>
@@ -5788,7 +5789,7 @@
         <v>#N/A</v>
       </c>
       <c r="G211" s="10"/>
-      <c r="H211" s="17"/>
+      <c r="H211" s="16"/>
       <c r="I211" s="10" t="e">
         <f t="shared" si="15"/>
         <v>#N/A</v>
@@ -5812,7 +5813,7 @@
         <v>#N/A</v>
       </c>
       <c r="G212" s="10"/>
-      <c r="H212" s="17"/>
+      <c r="H212" s="16"/>
       <c r="I212" s="10" t="e">
         <f t="shared" si="15"/>
         <v>#N/A</v>
@@ -5836,7 +5837,7 @@
         <v>#N/A</v>
       </c>
       <c r="G213" s="10"/>
-      <c r="H213" s="17"/>
+      <c r="H213" s="16"/>
       <c r="I213" s="10" t="e">
         <f t="shared" si="15"/>
         <v>#N/A</v>
@@ -5860,7 +5861,7 @@
         <v>#N/A</v>
       </c>
       <c r="G214" s="10"/>
-      <c r="H214" s="17"/>
+      <c r="H214" s="16"/>
       <c r="I214" s="10" t="e">
         <f t="shared" si="15"/>
         <v>#N/A</v>
@@ -5884,7 +5885,7 @@
         <v>#N/A</v>
       </c>
       <c r="G215" s="10"/>
-      <c r="H215" s="17"/>
+      <c r="H215" s="16"/>
       <c r="I215" s="10" t="e">
         <f t="shared" si="15"/>
         <v>#N/A</v>
@@ -5908,7 +5909,7 @@
         <v>#N/A</v>
       </c>
       <c r="G216" s="10"/>
-      <c r="H216" s="17"/>
+      <c r="H216" s="16"/>
       <c r="I216" s="10" t="e">
         <f t="shared" si="15"/>
         <v>#N/A</v>
@@ -5932,7 +5933,7 @@
         <v>#N/A</v>
       </c>
       <c r="G217" s="10"/>
-      <c r="H217" s="17"/>
+      <c r="H217" s="16"/>
       <c r="I217" s="10" t="e">
         <f t="shared" si="15"/>
         <v>#N/A</v>
@@ -5956,7 +5957,7 @@
         <v>#N/A</v>
       </c>
       <c r="G218" s="10"/>
-      <c r="H218" s="17"/>
+      <c r="H218" s="16"/>
       <c r="I218" s="10" t="e">
         <f t="shared" si="15"/>
         <v>#N/A</v>
@@ -5980,7 +5981,7 @@
         <v>#N/A</v>
       </c>
       <c r="G219" s="10"/>
-      <c r="H219" s="17"/>
+      <c r="H219" s="16"/>
       <c r="I219" s="10" t="e">
         <f t="shared" si="15"/>
         <v>#N/A</v>
@@ -6004,7 +6005,7 @@
         <v>#N/A</v>
       </c>
       <c r="G220" s="10"/>
-      <c r="H220" s="17"/>
+      <c r="H220" s="16"/>
       <c r="I220" s="10" t="e">
         <f t="shared" si="15"/>
         <v>#N/A</v>
@@ -6028,7 +6029,7 @@
         <v>#N/A</v>
       </c>
       <c r="G221" s="10"/>
-      <c r="H221" s="17"/>
+      <c r="H221" s="16"/>
       <c r="I221" s="10" t="e">
         <f t="shared" si="15"/>
         <v>#N/A</v>
@@ -6052,7 +6053,7 @@
         <v>#N/A</v>
       </c>
       <c r="G222" s="10"/>
-      <c r="H222" s="17"/>
+      <c r="H222" s="16"/>
       <c r="I222" s="10" t="e">
         <f t="shared" si="15"/>
         <v>#N/A</v>
@@ -6076,7 +6077,7 @@
         <v>#N/A</v>
       </c>
       <c r="G223" s="10"/>
-      <c r="H223" s="17"/>
+      <c r="H223" s="16"/>
       <c r="I223" s="10" t="e">
         <f t="shared" si="15"/>
         <v>#N/A</v>
@@ -6100,7 +6101,7 @@
         <v>#N/A</v>
       </c>
       <c r="G224" s="10"/>
-      <c r="H224" s="17"/>
+      <c r="H224" s="16"/>
       <c r="I224" s="10" t="e">
         <f t="shared" si="15"/>
         <v>#N/A</v>
@@ -6124,7 +6125,7 @@
         <v>#N/A</v>
       </c>
       <c r="G225" s="10"/>
-      <c r="H225" s="17"/>
+      <c r="H225" s="16"/>
       <c r="I225" s="10" t="e">
         <f t="shared" si="15"/>
         <v>#N/A</v>
@@ -6148,7 +6149,7 @@
         <v>#N/A</v>
       </c>
       <c r="G226" s="10"/>
-      <c r="H226" s="17"/>
+      <c r="H226" s="16"/>
       <c r="I226" s="10" t="e">
         <f t="shared" si="15"/>
         <v>#N/A</v>
@@ -6172,7 +6173,7 @@
         <v>#N/A</v>
       </c>
       <c r="G227" s="10"/>
-      <c r="H227" s="17"/>
+      <c r="H227" s="16"/>
       <c r="I227" s="10" t="e">
         <f t="shared" si="15"/>
         <v>#N/A</v>
@@ -6196,7 +6197,7 @@
         <v>#N/A</v>
       </c>
       <c r="G228" s="10"/>
-      <c r="H228" s="17"/>
+      <c r="H228" s="16"/>
       <c r="I228" s="10" t="e">
         <f t="shared" si="15"/>
         <v>#N/A</v>
@@ -6220,7 +6221,7 @@
         <v>#N/A</v>
       </c>
       <c r="G229" s="10"/>
-      <c r="H229" s="17"/>
+      <c r="H229" s="16"/>
       <c r="I229" s="10" t="e">
         <f t="shared" si="15"/>
         <v>#N/A</v>
@@ -6244,7 +6245,7 @@
         <v>#N/A</v>
       </c>
       <c r="G230" s="10"/>
-      <c r="H230" s="17"/>
+      <c r="H230" s="16"/>
       <c r="I230" s="10" t="e">
         <f t="shared" si="15"/>
         <v>#N/A</v>
@@ -6268,7 +6269,7 @@
         <v>#N/A</v>
       </c>
       <c r="G231" s="10"/>
-      <c r="H231" s="17"/>
+      <c r="H231" s="16"/>
       <c r="I231" s="10" t="e">
         <f t="shared" si="15"/>
         <v>#N/A</v>
@@ -6292,7 +6293,7 @@
         <v>#N/A</v>
       </c>
       <c r="G232" s="10"/>
-      <c r="H232" s="17"/>
+      <c r="H232" s="16"/>
       <c r="I232" s="10" t="e">
         <f t="shared" si="15"/>
         <v>#N/A</v>
@@ -6316,7 +6317,7 @@
         <v>#N/A</v>
       </c>
       <c r="G233" s="10"/>
-      <c r="H233" s="17"/>
+      <c r="H233" s="16"/>
       <c r="I233" s="10" t="e">
         <f t="shared" si="15"/>
         <v>#N/A</v>
@@ -6340,7 +6341,7 @@
         <v>#N/A</v>
       </c>
       <c r="G234" s="10"/>
-      <c r="H234" s="17"/>
+      <c r="H234" s="16"/>
       <c r="I234" s="10" t="e">
         <f t="shared" si="15"/>
         <v>#N/A</v>
@@ -6364,7 +6365,7 @@
         <v>#N/A</v>
       </c>
       <c r="G235" s="10"/>
-      <c r="H235" s="17"/>
+      <c r="H235" s="16"/>
       <c r="I235" s="10" t="e">
         <f t="shared" si="15"/>
         <v>#N/A</v>
@@ -6388,7 +6389,7 @@
         <v>#N/A</v>
       </c>
       <c r="G236" s="10"/>
-      <c r="H236" s="17"/>
+      <c r="H236" s="16"/>
       <c r="I236" s="10" t="e">
         <f t="shared" si="15"/>
         <v>#N/A</v>
@@ -6412,7 +6413,7 @@
         <v>#N/A</v>
       </c>
       <c r="G237" s="10"/>
-      <c r="H237" s="17"/>
+      <c r="H237" s="16"/>
       <c r="I237" s="10" t="e">
         <f t="shared" si="15"/>
         <v>#N/A</v>
@@ -6436,7 +6437,7 @@
         <v>#N/A</v>
       </c>
       <c r="G238" s="10"/>
-      <c r="H238" s="17"/>
+      <c r="H238" s="16"/>
       <c r="I238" s="10" t="e">
         <f t="shared" si="15"/>
         <v>#N/A</v>
@@ -6460,7 +6461,7 @@
         <v>#N/A</v>
       </c>
       <c r="G239" s="10"/>
-      <c r="H239" s="17"/>
+      <c r="H239" s="16"/>
       <c r="I239" s="10" t="e">
         <f t="shared" si="15"/>
         <v>#N/A</v>
@@ -6484,7 +6485,7 @@
         <v>#N/A</v>
       </c>
       <c r="G240" s="10"/>
-      <c r="H240" s="17"/>
+      <c r="H240" s="16"/>
       <c r="I240" s="10" t="e">
         <f t="shared" si="15"/>
         <v>#N/A</v>
@@ -6508,7 +6509,7 @@
         <v>#N/A</v>
       </c>
       <c r="G241" s="10"/>
-      <c r="H241" s="17"/>
+      <c r="H241" s="16"/>
       <c r="I241" s="10" t="e">
         <f t="shared" si="15"/>
         <v>#N/A</v>
@@ -6532,7 +6533,7 @@
         <v>#N/A</v>
       </c>
       <c r="G242" s="10"/>
-      <c r="H242" s="17"/>
+      <c r="H242" s="16"/>
       <c r="I242" s="10" t="e">
         <f t="shared" si="15"/>
         <v>#N/A</v>
@@ -6556,7 +6557,7 @@
         <v>#N/A</v>
       </c>
       <c r="G243" s="10"/>
-      <c r="H243" s="17"/>
+      <c r="H243" s="16"/>
       <c r="I243" s="10" t="e">
         <f t="shared" si="15"/>
         <v>#N/A</v>
@@ -6580,7 +6581,7 @@
         <v>#N/A</v>
       </c>
       <c r="G244" s="10"/>
-      <c r="H244" s="17"/>
+      <c r="H244" s="16"/>
       <c r="I244" s="10" t="e">
         <f t="shared" si="15"/>
         <v>#N/A</v>
@@ -6604,7 +6605,7 @@
         <v>#N/A</v>
       </c>
       <c r="G245" s="10"/>
-      <c r="H245" s="17"/>
+      <c r="H245" s="16"/>
       <c r="I245" s="10" t="e">
         <f t="shared" si="15"/>
         <v>#N/A</v>
@@ -6628,7 +6629,7 @@
         <v>#N/A</v>
       </c>
       <c r="G246" s="10"/>
-      <c r="H246" s="17"/>
+      <c r="H246" s="16"/>
       <c r="I246" s="10" t="e">
         <f t="shared" si="15"/>
         <v>#N/A</v>
@@ -6652,7 +6653,7 @@
         <v>#N/A</v>
       </c>
       <c r="G247" s="10"/>
-      <c r="H247" s="17"/>
+      <c r="H247" s="16"/>
       <c r="I247" s="10" t="e">
         <f t="shared" si="15"/>
         <v>#N/A</v>
@@ -6676,7 +6677,7 @@
         <v>#N/A</v>
       </c>
       <c r="G248" s="10"/>
-      <c r="H248" s="17"/>
+      <c r="H248" s="16"/>
       <c r="I248" s="10" t="e">
         <f t="shared" si="15"/>
         <v>#N/A</v>
@@ -6700,7 +6701,7 @@
         <v>#N/A</v>
       </c>
       <c r="G249" s="10"/>
-      <c r="H249" s="17"/>
+      <c r="H249" s="16"/>
       <c r="I249" s="10" t="e">
         <f t="shared" si="15"/>
         <v>#N/A</v>
@@ -6724,7 +6725,7 @@
         <v>#N/A</v>
       </c>
       <c r="G250" s="10"/>
-      <c r="H250" s="17"/>
+      <c r="H250" s="16"/>
       <c r="I250" s="10" t="e">
         <f t="shared" si="15"/>
         <v>#N/A</v>
@@ -6748,7 +6749,7 @@
         <v>#N/A</v>
       </c>
       <c r="G251" s="10"/>
-      <c r="H251" s="17"/>
+      <c r="H251" s="16"/>
       <c r="I251" s="10" t="e">
         <f t="shared" si="15"/>
         <v>#N/A</v>
@@ -6772,7 +6773,7 @@
         <v>#N/A</v>
       </c>
       <c r="G252" s="10"/>
-      <c r="H252" s="17"/>
+      <c r="H252" s="16"/>
       <c r="I252" s="10" t="e">
         <f t="shared" si="15"/>
         <v>#N/A</v>
@@ -6796,7 +6797,7 @@
         <v>#N/A</v>
       </c>
       <c r="G253" s="10"/>
-      <c r="H253" s="17"/>
+      <c r="H253" s="16"/>
       <c r="I253" s="10" t="e">
         <f t="shared" si="15"/>
         <v>#N/A</v>
@@ -6820,7 +6821,7 @@
         <v>#N/A</v>
       </c>
       <c r="G254" s="10"/>
-      <c r="H254" s="17"/>
+      <c r="H254" s="16"/>
       <c r="I254" s="10" t="e">
         <f t="shared" si="15"/>
         <v>#N/A</v>
@@ -6844,7 +6845,7 @@
         <v>#N/A</v>
       </c>
       <c r="G255" s="10"/>
-      <c r="H255" s="17"/>
+      <c r="H255" s="16"/>
       <c r="I255" s="10" t="e">
         <f t="shared" si="15"/>
         <v>#N/A</v>
@@ -6868,7 +6869,7 @@
         <v>#N/A</v>
       </c>
       <c r="G256" s="10"/>
-      <c r="H256" s="17"/>
+      <c r="H256" s="16"/>
       <c r="I256" s="10" t="e">
         <f t="shared" si="15"/>
         <v>#N/A</v>
@@ -6892,7 +6893,7 @@
         <v>#N/A</v>
       </c>
       <c r="G257" s="10"/>
-      <c r="H257" s="17"/>
+      <c r="H257" s="16"/>
       <c r="I257" s="10" t="e">
         <f t="shared" si="15"/>
         <v>#N/A</v>
@@ -6916,7 +6917,7 @@
         <v>#N/A</v>
       </c>
       <c r="G258" s="10"/>
-      <c r="H258" s="17"/>
+      <c r="H258" s="16"/>
       <c r="I258" s="10" t="e">
         <f t="shared" si="15"/>
         <v>#N/A</v>
@@ -6940,7 +6941,7 @@
         <v>#N/A</v>
       </c>
       <c r="G259" s="10"/>
-      <c r="H259" s="17"/>
+      <c r="H259" s="16"/>
       <c r="I259" s="10" t="e">
         <f t="shared" ref="I259:I310" si="19">VLOOKUP(J259,Tabla_Mes,2,)</f>
         <v>#N/A</v>
@@ -6964,7 +6965,7 @@
         <v>#N/A</v>
       </c>
       <c r="G260" s="10"/>
-      <c r="H260" s="17"/>
+      <c r="H260" s="16"/>
       <c r="I260" s="10" t="e">
         <f t="shared" si="19"/>
         <v>#N/A</v>
@@ -6988,7 +6989,7 @@
         <v>#N/A</v>
       </c>
       <c r="G261" s="10"/>
-      <c r="H261" s="17"/>
+      <c r="H261" s="16"/>
       <c r="I261" s="10" t="e">
         <f t="shared" si="19"/>
         <v>#N/A</v>
@@ -7012,7 +7013,7 @@
         <v>#N/A</v>
       </c>
       <c r="G262" s="10"/>
-      <c r="H262" s="17"/>
+      <c r="H262" s="16"/>
       <c r="I262" s="10" t="e">
         <f t="shared" si="19"/>
         <v>#N/A</v>
@@ -7036,7 +7037,7 @@
         <v>#N/A</v>
       </c>
       <c r="G263" s="10"/>
-      <c r="H263" s="17"/>
+      <c r="H263" s="16"/>
       <c r="I263" s="10" t="e">
         <f t="shared" si="19"/>
         <v>#N/A</v>
@@ -7060,7 +7061,7 @@
         <v>#N/A</v>
       </c>
       <c r="G264" s="10"/>
-      <c r="H264" s="17"/>
+      <c r="H264" s="16"/>
       <c r="I264" s="10" t="e">
         <f t="shared" si="19"/>
         <v>#N/A</v>
@@ -7084,7 +7085,7 @@
         <v>#N/A</v>
       </c>
       <c r="G265" s="10"/>
-      <c r="H265" s="17"/>
+      <c r="H265" s="16"/>
       <c r="I265" s="10" t="e">
         <f t="shared" si="19"/>
         <v>#N/A</v>
@@ -7108,7 +7109,7 @@
         <v>#N/A</v>
       </c>
       <c r="G266" s="10"/>
-      <c r="H266" s="17"/>
+      <c r="H266" s="16"/>
       <c r="I266" s="10" t="e">
         <f t="shared" si="19"/>
         <v>#N/A</v>
@@ -7132,7 +7133,7 @@
         <v>#N/A</v>
       </c>
       <c r="G267" s="10"/>
-      <c r="H267" s="17"/>
+      <c r="H267" s="16"/>
       <c r="I267" s="10" t="e">
         <f t="shared" si="19"/>
         <v>#N/A</v>
@@ -7156,7 +7157,7 @@
         <v>#N/A</v>
       </c>
       <c r="G268" s="10"/>
-      <c r="H268" s="17"/>
+      <c r="H268" s="16"/>
       <c r="I268" s="10" t="e">
         <f t="shared" si="19"/>
         <v>#N/A</v>
@@ -7180,7 +7181,7 @@
         <v>#N/A</v>
       </c>
       <c r="G269" s="10"/>
-      <c r="H269" s="17"/>
+      <c r="H269" s="16"/>
       <c r="I269" s="10" t="e">
         <f t="shared" si="19"/>
         <v>#N/A</v>
@@ -7204,7 +7205,7 @@
         <v>#N/A</v>
       </c>
       <c r="G270" s="10"/>
-      <c r="H270" s="17"/>
+      <c r="H270" s="16"/>
       <c r="I270" s="10" t="e">
         <f t="shared" si="19"/>
         <v>#N/A</v>
@@ -7228,7 +7229,7 @@
         <v>#N/A</v>
       </c>
       <c r="G271" s="10"/>
-      <c r="H271" s="17"/>
+      <c r="H271" s="16"/>
       <c r="I271" s="10" t="e">
         <f t="shared" si="19"/>
         <v>#N/A</v>
@@ -7252,7 +7253,7 @@
         <v>#N/A</v>
       </c>
       <c r="G272" s="10"/>
-      <c r="H272" s="17"/>
+      <c r="H272" s="16"/>
       <c r="I272" s="10" t="e">
         <f t="shared" si="19"/>
         <v>#N/A</v>
@@ -7276,7 +7277,7 @@
         <v>#N/A</v>
       </c>
       <c r="G273" s="10"/>
-      <c r="H273" s="17"/>
+      <c r="H273" s="16"/>
       <c r="I273" s="10" t="e">
         <f t="shared" si="19"/>
         <v>#N/A</v>
@@ -7300,7 +7301,7 @@
         <v>#N/A</v>
       </c>
       <c r="G274" s="10"/>
-      <c r="H274" s="17"/>
+      <c r="H274" s="16"/>
       <c r="I274" s="10" t="e">
         <f t="shared" si="19"/>
         <v>#N/A</v>
@@ -7324,7 +7325,7 @@
         <v>#N/A</v>
       </c>
       <c r="G275" s="10"/>
-      <c r="H275" s="17"/>
+      <c r="H275" s="16"/>
       <c r="I275" s="10" t="e">
         <f t="shared" si="19"/>
         <v>#N/A</v>
@@ -7348,7 +7349,7 @@
         <v>#N/A</v>
       </c>
       <c r="G276" s="10"/>
-      <c r="H276" s="17"/>
+      <c r="H276" s="16"/>
       <c r="I276" s="10" t="e">
         <f t="shared" si="19"/>
         <v>#N/A</v>
@@ -7372,7 +7373,7 @@
         <v>#N/A</v>
       </c>
       <c r="G277" s="10"/>
-      <c r="H277" s="17"/>
+      <c r="H277" s="16"/>
       <c r="I277" s="10" t="e">
         <f t="shared" si="19"/>
         <v>#N/A</v>
@@ -7396,7 +7397,7 @@
         <v>#N/A</v>
       </c>
       <c r="G278" s="10"/>
-      <c r="H278" s="17"/>
+      <c r="H278" s="16"/>
       <c r="I278" s="10" t="e">
         <f t="shared" si="19"/>
         <v>#N/A</v>
@@ -7420,7 +7421,7 @@
         <v>#N/A</v>
       </c>
       <c r="G279" s="10"/>
-      <c r="H279" s="17"/>
+      <c r="H279" s="16"/>
       <c r="I279" s="10" t="e">
         <f t="shared" si="19"/>
         <v>#N/A</v>
@@ -7444,7 +7445,7 @@
         <v>#N/A</v>
       </c>
       <c r="G280" s="10"/>
-      <c r="H280" s="17"/>
+      <c r="H280" s="16"/>
       <c r="I280" s="10" t="e">
         <f t="shared" si="19"/>
         <v>#N/A</v>
@@ -7468,7 +7469,7 @@
         <v>#N/A</v>
       </c>
       <c r="G281" s="10"/>
-      <c r="H281" s="17"/>
+      <c r="H281" s="16"/>
       <c r="I281" s="10" t="e">
         <f t="shared" si="19"/>
         <v>#N/A</v>
@@ -7492,7 +7493,7 @@
         <v>#N/A</v>
       </c>
       <c r="G282" s="10"/>
-      <c r="H282" s="17"/>
+      <c r="H282" s="16"/>
       <c r="I282" s="10" t="e">
         <f t="shared" si="19"/>
         <v>#N/A</v>
@@ -7516,7 +7517,7 @@
         <v>#N/A</v>
       </c>
       <c r="G283" s="10"/>
-      <c r="H283" s="17"/>
+      <c r="H283" s="16"/>
       <c r="I283" s="10" t="e">
         <f t="shared" si="19"/>
         <v>#N/A</v>
@@ -7540,7 +7541,7 @@
         <v>#N/A</v>
       </c>
       <c r="G284" s="10"/>
-      <c r="H284" s="17"/>
+      <c r="H284" s="16"/>
       <c r="I284" s="10" t="e">
         <f t="shared" si="19"/>
         <v>#N/A</v>
@@ -7564,7 +7565,7 @@
         <v>#N/A</v>
       </c>
       <c r="G285" s="10"/>
-      <c r="H285" s="17"/>
+      <c r="H285" s="16"/>
       <c r="I285" s="10" t="e">
         <f t="shared" si="19"/>
         <v>#N/A</v>
@@ -7588,7 +7589,7 @@
         <v>#N/A</v>
       </c>
       <c r="G286" s="10"/>
-      <c r="H286" s="17"/>
+      <c r="H286" s="16"/>
       <c r="I286" s="10" t="e">
         <f t="shared" si="19"/>
         <v>#N/A</v>
@@ -7612,7 +7613,7 @@
         <v>#N/A</v>
       </c>
       <c r="G287" s="10"/>
-      <c r="H287" s="17"/>
+      <c r="H287" s="16"/>
       <c r="I287" s="10" t="e">
         <f t="shared" si="19"/>
         <v>#N/A</v>
@@ -7636,7 +7637,7 @@
         <v>#N/A</v>
       </c>
       <c r="G288" s="10"/>
-      <c r="H288" s="17"/>
+      <c r="H288" s="16"/>
       <c r="I288" s="10" t="e">
         <f t="shared" si="19"/>
         <v>#N/A</v>
@@ -7660,7 +7661,7 @@
         <v>#N/A</v>
       </c>
       <c r="G289" s="10"/>
-      <c r="H289" s="17"/>
+      <c r="H289" s="16"/>
       <c r="I289" s="10" t="e">
         <f t="shared" si="19"/>
         <v>#N/A</v>
@@ -7684,7 +7685,7 @@
         <v>#N/A</v>
       </c>
       <c r="G290" s="10"/>
-      <c r="H290" s="17"/>
+      <c r="H290" s="16"/>
       <c r="I290" s="10" t="e">
         <f t="shared" si="19"/>
         <v>#N/A</v>
@@ -7708,7 +7709,7 @@
         <v>#N/A</v>
       </c>
       <c r="G291" s="10"/>
-      <c r="H291" s="17"/>
+      <c r="H291" s="16"/>
       <c r="I291" s="10" t="e">
         <f t="shared" si="19"/>
         <v>#N/A</v>
@@ -7732,7 +7733,7 @@
         <v>#N/A</v>
       </c>
       <c r="G292" s="10"/>
-      <c r="H292" s="17"/>
+      <c r="H292" s="16"/>
       <c r="I292" s="10" t="e">
         <f t="shared" si="19"/>
         <v>#N/A</v>
@@ -7756,7 +7757,7 @@
         <v>#N/A</v>
       </c>
       <c r="G293" s="10"/>
-      <c r="H293" s="17"/>
+      <c r="H293" s="16"/>
       <c r="I293" s="10" t="e">
         <f t="shared" si="19"/>
         <v>#N/A</v>
@@ -7780,7 +7781,7 @@
         <v>#N/A</v>
       </c>
       <c r="G294" s="10"/>
-      <c r="H294" s="17"/>
+      <c r="H294" s="16"/>
       <c r="I294" s="10" t="e">
         <f t="shared" si="19"/>
         <v>#N/A</v>
@@ -7804,7 +7805,7 @@
         <v>#N/A</v>
       </c>
       <c r="G295" s="10"/>
-      <c r="H295" s="17"/>
+      <c r="H295" s="16"/>
       <c r="I295" s="10" t="e">
         <f t="shared" si="19"/>
         <v>#N/A</v>
@@ -7828,7 +7829,7 @@
         <v>#N/A</v>
       </c>
       <c r="G296" s="10"/>
-      <c r="H296" s="17"/>
+      <c r="H296" s="16"/>
       <c r="I296" s="10" t="e">
         <f t="shared" si="19"/>
         <v>#N/A</v>
@@ -7852,7 +7853,7 @@
         <v>#N/A</v>
       </c>
       <c r="G297" s="10"/>
-      <c r="H297" s="17"/>
+      <c r="H297" s="16"/>
       <c r="I297" s="10" t="e">
         <f t="shared" si="19"/>
         <v>#N/A</v>
@@ -7876,7 +7877,7 @@
         <v>#N/A</v>
       </c>
       <c r="G298" s="10"/>
-      <c r="H298" s="17"/>
+      <c r="H298" s="16"/>
       <c r="I298" s="10" t="e">
         <f t="shared" si="19"/>
         <v>#N/A</v>
@@ -7900,7 +7901,7 @@
         <v>#N/A</v>
       </c>
       <c r="G299" s="10"/>
-      <c r="H299" s="17"/>
+      <c r="H299" s="16"/>
       <c r="I299" s="10" t="e">
         <f t="shared" si="19"/>
         <v>#N/A</v>
@@ -7924,7 +7925,7 @@
         <v>#N/A</v>
       </c>
       <c r="G300" s="10"/>
-      <c r="H300" s="17"/>
+      <c r="H300" s="16"/>
       <c r="I300" s="10" t="e">
         <f t="shared" si="19"/>
         <v>#N/A</v>
@@ -7948,7 +7949,7 @@
         <v>#N/A</v>
       </c>
       <c r="G301" s="10"/>
-      <c r="H301" s="17"/>
+      <c r="H301" s="16"/>
       <c r="I301" s="10" t="e">
         <f t="shared" si="19"/>
         <v>#N/A</v>
@@ -7972,7 +7973,7 @@
         <v>#N/A</v>
       </c>
       <c r="G302" s="10"/>
-      <c r="H302" s="17"/>
+      <c r="H302" s="16"/>
       <c r="I302" s="10" t="e">
         <f t="shared" si="19"/>
         <v>#N/A</v>
@@ -7996,7 +7997,7 @@
         <v>#N/A</v>
       </c>
       <c r="G303" s="10"/>
-      <c r="H303" s="17"/>
+      <c r="H303" s="16"/>
       <c r="I303" s="10" t="e">
         <f t="shared" si="19"/>
         <v>#N/A</v>
@@ -8020,7 +8021,7 @@
         <v>#N/A</v>
       </c>
       <c r="G304" s="10"/>
-      <c r="H304" s="17"/>
+      <c r="H304" s="16"/>
       <c r="I304" s="10" t="e">
         <f t="shared" si="19"/>
         <v>#N/A</v>
@@ -8044,7 +8045,7 @@
         <v>#N/A</v>
       </c>
       <c r="G305" s="10"/>
-      <c r="H305" s="17"/>
+      <c r="H305" s="16"/>
       <c r="I305" s="10" t="e">
         <f t="shared" si="19"/>
         <v>#N/A</v>
@@ -8068,7 +8069,7 @@
         <v>#N/A</v>
       </c>
       <c r="G306" s="10"/>
-      <c r="H306" s="17"/>
+      <c r="H306" s="16"/>
       <c r="I306" s="10" t="e">
         <f t="shared" si="19"/>
         <v>#N/A</v>
@@ -8092,7 +8093,7 @@
         <v>#N/A</v>
       </c>
       <c r="G307" s="10"/>
-      <c r="H307" s="17"/>
+      <c r="H307" s="16"/>
       <c r="I307" s="10" t="e">
         <f t="shared" si="19"/>
         <v>#N/A</v>
@@ -8116,7 +8117,7 @@
         <v>#N/A</v>
       </c>
       <c r="G308" s="10"/>
-      <c r="H308" s="17"/>
+      <c r="H308" s="16"/>
       <c r="I308" s="10" t="e">
         <f t="shared" si="19"/>
         <v>#N/A</v>
@@ -8140,7 +8141,7 @@
         <v>#N/A</v>
       </c>
       <c r="G309" s="10"/>
-      <c r="H309" s="17"/>
+      <c r="H309" s="16"/>
       <c r="I309" s="10" t="e">
         <f t="shared" si="19"/>
         <v>#N/A</v>
@@ -8164,7 +8165,7 @@
         <v>#N/A</v>
       </c>
       <c r="G310" s="10"/>
-      <c r="H310" s="17"/>
+      <c r="H310" s="16"/>
       <c r="I310" s="10" t="e">
         <f t="shared" si="19"/>
         <v>#N/A</v>
@@ -8172,10 +8173,10 @@
       <c r="J310" s="10"/>
     </row>
     <row r="311" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="H311" s="17"/>
+      <c r="H311" s="16"/>
     </row>
   </sheetData>
-  <sheetProtection algorithmName="SHA-512" hashValue="Yr1oDB68Mhcj+iA4VyJVNDCu8FviVr3iO5YLjjKhLictro/7tHyWkOioWWWyrAczYGdpHww5wr9h4eUQOl2U3A==" saltValue="nLIMP2xWImcZnvpRq4/kYg==" spinCount="100000" sheet="1" objects="1" scenarios="1" selectLockedCells="1"/>
+  <sheetProtection algorithmName="SHA-512" hashValue="Jh+eKDozn8JSBu0KIHX1M/PixmOReSy4FKBaA66gT4UY0iB/sMdvhqsSAb14+IL//C39Kncm1LC3ECHgX9nxKg==" saltValue="V4GYMc+2lzwr8etLNJinCg==" spinCount="100000" sheet="1" objects="1" scenarios="1" selectLockedCells="1"/>
   <dataValidations count="7">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A3:A310" xr:uid="{ECE28117-C8FA-4388-B6C8-4DC009C7D8F9}">
       <formula1>Lista_Anno</formula1>
@@ -8357,8 +8358,8 @@
       <c r="A11" s="6">
         <v>2016</v>
       </c>
-      <c r="C11" s="14"/>
-      <c r="D11" s="14"/>
+      <c r="C11" s="13"/>
+      <c r="D11" s="13"/>
       <c r="F11" s="7" t="s">
         <v>13</v>
       </c>
@@ -8382,8 +8383,8 @@
       <c r="A12" s="6">
         <v>2017</v>
       </c>
-      <c r="C12" s="14"/>
-      <c r="D12" s="14"/>
+      <c r="C12" s="13"/>
+      <c r="D12" s="13"/>
       <c r="F12" s="7" t="s">
         <v>14</v>
       </c>

</xml_diff>